<commit_message>
adding lab8 guide and IPAM update
</commit_message>
<xml_diff>
--- a/Lab1_Network_Infrastructure_Imeplementation/IPAM.xlsx
+++ b/Lab1_Network_Infrastructure_Imeplementation/IPAM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Coursework\CSCI_5840_Adv_Net_Man\Lab1_Network_Infrastructure_Imeplementation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E912933E-4A1A-4923-ADDE-1CACB294EBC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CABF9149-C089-4CA6-BB2F-81AC8416BF9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26715" yWindow="1530" windowWidth="10305" windowHeight="18405" xr2:uid="{16A71B2A-6EEC-4485-B5DE-3118DDB1AB7E}"/>
+    <workbookView xWindow="-11205" yWindow="4080" windowWidth="10200" windowHeight="13425" xr2:uid="{16A71B2A-6EEC-4485-B5DE-3118DDB1AB7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="105">
   <si>
     <t>VLAN10_CUST</t>
   </si>
@@ -297,6 +297,60 @@
   </si>
   <si>
     <t>2404::/64</t>
+  </si>
+  <si>
+    <t>H5</t>
+  </si>
+  <si>
+    <t>2.2.2.2/30</t>
+  </si>
+  <si>
+    <t>2222::2/64</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>eth4</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>2.2.2.1/30</t>
+  </si>
+  <si>
+    <t>2222::1/64</t>
+  </si>
+  <si>
+    <t>2666::1/64</t>
+  </si>
+  <si>
+    <t>2666::2/64</t>
+  </si>
+  <si>
+    <t>2777::1/64</t>
+  </si>
+  <si>
+    <t>2777::2/64</t>
+  </si>
+  <si>
+    <t>10.40.100.1/24</t>
+  </si>
+  <si>
+    <t>10.40.101.2/24</t>
+  </si>
+  <si>
+    <t>10.40.100.2/24</t>
+  </si>
+  <si>
+    <t>10.40.101.1/24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R6 </t>
+  </si>
+  <si>
+    <t>10.40.6.1/32</t>
   </si>
 </sst>
 </file>
@@ -668,10 +722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3591833E-9C2C-4F06-A62C-CC6A3D65A3CF}">
-  <dimension ref="A1:Q36"/>
+  <dimension ref="A1:Q44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1109,17 +1163,17 @@
         <v>86</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>23</v>
       </c>
@@ -1130,7 +1184,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>24</v>
       </c>
@@ -1139,6 +1193,101 @@
       </c>
       <c r="C36" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>87</v>
+      </c>
+      <c r="B38" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" t="s">
+        <v>88</v>
+      </c>
+      <c r="D38" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>90</v>
+      </c>
+      <c r="B39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" t="s">
+        <v>101</v>
+      </c>
+      <c r="D39" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" t="s">
+        <v>91</v>
+      </c>
+      <c r="C40" t="s">
+        <v>99</v>
+      </c>
+      <c r="D40" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>90</v>
+      </c>
+      <c r="B41" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" t="s">
+        <v>102</v>
+      </c>
+      <c r="D41" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>92</v>
+      </c>
+      <c r="B42" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" t="s">
+        <v>100</v>
+      </c>
+      <c r="D42" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>92</v>
+      </c>
+      <c r="B43" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" t="s">
+        <v>93</v>
+      </c>
+      <c r="D43" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>103</v>
+      </c>
+      <c r="B44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>